<commit_message>
cleaned up state name spaces
</commit_message>
<xml_diff>
--- a/PeopleStates.xlsx
+++ b/PeopleStates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -69,160 +69,157 @@
     <t>state</t>
   </si>
   <si>
-    <t xml:space="preserve"> California</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Texas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Florida</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New York</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Illinois</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pennsylvania</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ohio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Georgia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> North Carolina</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Michigan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New Jersey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Virginia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Washington</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Arizona</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Massachusetts</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tennessee</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Indiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Missouri</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maryland</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wisconsin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Colorado</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Minnesota</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> South Carolina</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alabama</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Louisiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kentucky</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oregon</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oklahoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Connecticut</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Iowa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Utah</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mississippi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Arkansas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nevada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kansas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nebraska</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> West Virginia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Idaho</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hawaii</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New Hampshire</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Maine</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Rhode Island</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Montana</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Delaware</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> South Dakota</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  North Dakota</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Alaska</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vermont</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wyoming</t>
-  </si>
-  <si>
     <t>population_2010</t>
   </si>
   <si>
     <t>house_seats</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
   </si>
 </sst>
 </file>
@@ -540,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -603,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -618,15 +615,15 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>37254503</v>
@@ -637,7 +634,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>25146105</v>
@@ -648,7 +645,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>18804623</v>
@@ -659,7 +656,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1">
         <v>19378087</v>
@@ -670,7 +667,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>12831549</v>
@@ -681,7 +678,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>12702887</v>
@@ -692,7 +689,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>11536725</v>
@@ -703,7 +700,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
         <v>9688681</v>
@@ -714,7 +711,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1">
         <v>9535692</v>
@@ -725,7 +722,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1">
         <v>9884129</v>
@@ -736,7 +733,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>8791936</v>
@@ -747,7 +744,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1">
         <v>8001045</v>
@@ -758,7 +755,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1">
         <v>6724543</v>
@@ -769,7 +766,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>6392307</v>
@@ -780,7 +777,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1">
         <v>6547817</v>
@@ -791,7 +788,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>6346275</v>
@@ -802,7 +799,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1">
         <v>6484229</v>
@@ -813,7 +810,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1">
         <v>5988927</v>
@@ -824,7 +821,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1">
         <v>5773785</v>
@@ -835,7 +832,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1">
         <v>5687289</v>
@@ -846,7 +843,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1">
         <v>5029324</v>
@@ -857,7 +854,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1">
         <v>5303925</v>
@@ -868,7 +865,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1">
         <v>4625401</v>
@@ -879,7 +876,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1">
         <v>4780127</v>
@@ -890,7 +887,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1">
         <v>4533479</v>
@@ -901,7 +898,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1">
         <v>4339349</v>
@@ -912,7 +909,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1">
         <v>3831073</v>
@@ -923,7 +920,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1">
         <v>3751616</v>
@@ -934,7 +931,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1">
         <v>3574118</v>
@@ -945,7 +942,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1">
         <v>3046869</v>
@@ -956,7 +953,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B32" s="1">
         <v>2763888</v>
@@ -967,7 +964,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1">
         <v>2968103</v>
@@ -978,7 +975,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1">
         <v>2915958</v>
@@ -989,7 +986,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1">
         <v>2700691</v>
@@ -1000,7 +997,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1">
         <v>2853132</v>
@@ -1011,7 +1008,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B37" s="1">
         <v>2059192</v>
@@ -1022,7 +1019,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B38" s="1">
         <v>1826341</v>
@@ -1033,7 +1030,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B39" s="1">
         <v>1853011</v>
@@ -1044,7 +1041,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1">
         <v>1567652</v>
@@ -1055,7 +1052,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1">
         <v>1360301</v>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1">
         <v>1316466</v>
@@ -1077,7 +1074,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B43" s="1">
         <v>1328361</v>
@@ -1088,7 +1085,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B44" s="1">
         <v>1052931</v>
@@ -1099,7 +1096,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B45" s="1">
         <v>989417</v>
@@ -1110,7 +1107,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B46" s="1">
         <v>897936</v>
@@ -1121,7 +1118,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="B47" s="1">
         <v>814191</v>
@@ -1132,7 +1129,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B48" s="1">
         <v>672591</v>
@@ -1143,7 +1140,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B49" s="1">
         <v>710249</v>
@@ -1154,7 +1151,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B50" s="1">
         <v>625745</v>
@@ -1165,7 +1162,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B51" s="1">
         <v>563767</v>

</xml_diff>

<commit_message>
cleaned up state comma spaces
</commit_message>
<xml_diff>
--- a/PeopleStates.xlsx
+++ b/PeopleStates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,21 +39,12 @@
     <t>Bobby</t>
   </si>
   <si>
-    <t>Wyoming, Michigan</t>
-  </si>
-  <si>
     <t>Sue</t>
   </si>
   <si>
-    <t>Wisconsin, Nevada, California</t>
-  </si>
-  <si>
     <t>Tamika</t>
   </si>
   <si>
-    <t>Florida, Washington</t>
-  </si>
-  <si>
     <t>Cale</t>
   </si>
   <si>
@@ -63,9 +54,6 @@
     <t>Iris</t>
   </si>
   <si>
-    <t>Washington, Oregon, California</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -220,6 +208,18 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Wyoming,Michigan</t>
+  </si>
+  <si>
+    <t>Wisconsin,Nevada,California</t>
+  </si>
+  <si>
+    <t>Florida,Washington</t>
+  </si>
+  <si>
+    <t>Washington,Oregon,California</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,39 +556,39 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
@@ -612,18 +612,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>37254503</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>25146105</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>18804623</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>19378087</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>12831549</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>12702887</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>11536725</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>9688681</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>9535692</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1">
         <v>9884129</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>8791936</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
         <v>8001045</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
         <v>6724543</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
         <v>6392307</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1">
         <v>6547817</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>6346275</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1">
         <v>6484229</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1">
         <v>5988927</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1">
         <v>5773785</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1">
         <v>5687289</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>5029324</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
         <v>5303925</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1">
         <v>4625401</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1">
         <v>4780127</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1">
         <v>4533479</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1">
         <v>4339349</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1">
         <v>3831073</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1">
         <v>3751616</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1">
         <v>3574118</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>3046869</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1">
         <v>2763888</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1">
         <v>2968103</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1">
         <v>2915958</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1">
         <v>2700691</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1">
         <v>2853132</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1">
         <v>2059192</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1">
         <v>1826341</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1">
         <v>1853011</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1">
         <v>1567652</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1">
         <v>1360301</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B42" s="1">
         <v>1316466</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B43" s="1">
         <v>1328361</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1">
         <v>1052931</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1">
         <v>989417</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1">
         <v>897936</v>
@@ -1118,7 +1118,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1">
         <v>814191</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B48" s="1">
         <v>672591</v>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1">
         <v>710249</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B50" s="1">
         <v>625745</v>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B51" s="1">
         <v>563767</v>

</xml_diff>